<commit_message>
updated extract_outlets to scrape services
</commit_message>
<xml_diff>
--- a/backend/outlets.xlsx
+++ b/backend/outlets.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,11 @@
           <t>Longitude</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Services</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -492,6 +497,11 @@
       <c r="F2" t="n">
         <v>101.710931</v>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>24 Hours, Birthday Party, Breakfast, Cashless Facility, McCafe, McDelivery, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -520,6 +530,11 @@
       <c r="F3" t="n">
         <v>101.672297</v>
       </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>24 Hours, Birthday Party, Breakfast, Cashless Facility, McCafe, McDelivery, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -548,6 +563,11 @@
       <c r="F4" t="n">
         <v>101.734244</v>
       </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Birthday Party, Breakfast, Cashless Facility, Dessert Center, McCafe, McDelivery, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -576,6 +596,11 @@
       <c r="F5" t="n">
         <v>101.74152</v>
       </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>24 Hours, Birthday Party, Breakfast, Cashless Facility, McCafe, McDelivery, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -604,6 +629,11 @@
       <c r="F6" t="n">
         <v>101.736853</v>
       </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Birthday Party, Cashless Facility, Dessert Center, McCafe, McDelivery, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -632,6 +662,11 @@
       <c r="F7" t="n">
         <v>101.696865</v>
       </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Birthday Party, Breakfast, Cashless Facility, McCafe, McDelivery, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -660,6 +695,11 @@
       <c r="F8" t="n">
         <v>101.711531</v>
       </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Birthday Party, Breakfast, Cashless Facility, McCafe, McDelivery, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -688,6 +728,11 @@
       <c r="F9" t="n">
         <v>101.652203</v>
       </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Birthday Party, Drive-Thru, Breakfast, Cashless Facility, McCafe, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -716,6 +761,11 @@
       <c r="F10" t="n">
         <v>101.705739</v>
       </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Birthday Party, Cashless Facility, Dessert Center, McCafe, McDelivery, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -744,6 +794,11 @@
       <c r="F11" t="n">
         <v>101.607767</v>
       </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Birthday Party, Drive-Thru, Breakfast, Cashless Facility, McCafe, McDelivery, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -772,6 +827,11 @@
       <c r="F12" t="n">
         <v>101.762843</v>
       </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Birthday Party, Drive-Thru, Breakfast, Cashless Facility, McCafe, McDelivery, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -800,6 +860,11 @@
       <c r="F13" t="n">
         <v>101.743585</v>
       </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Birthday Party, Drive-Thru, Breakfast, Cashless Facility, McCafe, McDelivery, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -828,6 +893,11 @@
       <c r="F14" t="n">
         <v>101.710819</v>
       </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Birthday Party, Drive-Thru, Breakfast, Cashless Facility, McCafe, McDelivery, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -856,6 +926,11 @@
       <c r="F15" t="n">
         <v>101.690106</v>
       </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>24 Hours, Birthday Party, Drive-Thru, Breakfast, Cashless Facility, McCafe, McDelivery, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -884,6 +959,11 @@
       <c r="F16" t="n">
         <v>101.731946</v>
       </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>24 Hours, Birthday Party, Drive-Thru, Breakfast, Cashless Facility, McCafe, McDelivery, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -912,6 +992,11 @@
       <c r="F17" t="n">
         <v>101.704186</v>
       </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Birthday Party, Breakfast, Cashless Facility, Dessert Center, McCafe, McDelivery, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -940,6 +1025,11 @@
       <c r="F18" t="n">
         <v>101.728649</v>
       </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Birthday Party, Drive-Thru, Breakfast, Cashless Facility, McCafe, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -968,6 +1058,11 @@
       <c r="F19" t="n">
         <v>101.732853</v>
       </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>24 Hours, Birthday Party, Breakfast, Cashless Facility, Dessert Center, McCafe, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -996,6 +1091,11 @@
       <c r="F20" t="n">
         <v>101.65503</v>
       </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>24 Hours, Birthday Party, Drive-Thru, Breakfast, Cashless Facility, McCafe, McDelivery, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1024,6 +1124,11 @@
       <c r="F21" t="n">
         <v>101.695732</v>
       </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>24 Hours, Birthday Party, Drive-Thru, Breakfast, Cashless Facility, McDelivery, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1052,6 +1157,11 @@
       <c r="F22" t="n">
         <v>101.629209</v>
       </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Birthday Party, Breakfast, Cashless Facility, McCafe, McDelivery, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1080,6 +1190,11 @@
       <c r="F23" t="n">
         <v>101.735889</v>
       </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Birthday Party, Drive-Thru, Breakfast, Cashless Facility, McCafe, McDelivery, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1108,6 +1223,11 @@
       <c r="F24" t="n">
         <v>101.687277</v>
       </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Birthday Party, Cashless Facility, Dessert Center, McCafe, McDelivery, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1136,6 +1256,11 @@
       <c r="F25" t="n">
         <v>101.6918</v>
       </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>24 Hours, Birthday Party, Breakfast, Cashless Facility, McCafe, McDelivery, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1164,6 +1289,11 @@
       <c r="F26" t="n">
         <v>101.677572</v>
       </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Birthday Party, Cashless Facility, Dessert Center, McCafe, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1192,6 +1322,11 @@
       <c r="F27" t="n">
         <v>101.686593</v>
       </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Birthday Party, Breakfast, Cashless Facility, Dessert Center, McCafe, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1220,6 +1355,11 @@
       <c r="F28" t="n">
         <v>101.712164</v>
       </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Birthday Party, Breakfast, Cashless Facility, Dessert Center, McCafe, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1248,6 +1388,11 @@
       <c r="F29" t="n">
         <v>101.723645</v>
       </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Birthday Party, Cashless Facility, Dessert Center, McCafe, McDelivery, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1276,6 +1421,11 @@
       <c r="F30" t="n">
         <v>101.724463</v>
       </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Birthday Party, Cashless Facility, Dessert Center, McCafe, McDelivery, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1304,6 +1454,11 @@
       <c r="F31" t="n">
         <v>101.720181</v>
       </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Birthday Party, Breakfast, Cashless Facility, Dessert Center, McCafe, McDelivery, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1332,6 +1487,11 @@
       <c r="F32" t="n">
         <v>101.7175568</v>
       </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>24 Hours, Birthday Party, Drive-Thru, Breakfast, Cashless Facility, McCafe, McDelivery, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1360,6 +1520,11 @@
       <c r="F33" t="n">
         <v>101.62778</v>
       </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>24 Hours, Birthday Party, Drive-Thru, Breakfast, Cashless Facility, McCafe, McDelivery, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1388,6 +1553,11 @@
       <c r="F34" t="n">
         <v>101.673568</v>
       </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>24 Hours, Birthday Party, Drive-Thru, Breakfast, Cashless Facility, McCafe, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1416,6 +1586,11 @@
       <c r="F35" t="n">
         <v>101.708461</v>
       </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>24 Hours, Birthday Party, Breakfast, Cashless Facility, McCafe, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1444,6 +1619,11 @@
       <c r="F36" t="n">
         <v>101.653579</v>
       </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>24 Hours, Birthday Party, Drive-Thru, Breakfast, Cashless Facility, McCafe, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1472,6 +1652,11 @@
       <c r="F37" t="n">
         <v>101.41208</v>
       </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Birthday Party, Drive-Thru, Breakfast, Cashless Facility, McCafe, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1500,6 +1685,11 @@
       <c r="F38" t="n">
         <v>101.42334</v>
       </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>24 Hours, Birthday Party, Breakfast, Cashless Facility, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1528,6 +1718,11 @@
       <c r="F39" t="n">
         <v>101.689976</v>
       </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Birthday Party, Drive-Thru, Breakfast, Cashless Facility, McCafe, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1556,6 +1751,11 @@
       <c r="F40" t="n">
         <v>101.745321</v>
       </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Drive-Thru, Breakfast, Cashless Facility, McCafe, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1584,6 +1784,11 @@
       <c r="F41" t="n">
         <v>101.7178428</v>
       </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Drive-Thru, Breakfast, Cashless Facility, McCafe, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1608,6 +1813,11 @@
       <c r="F42" t="n">
         <v>101.6721257</v>
       </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Drive-Thru, Breakfast, Cashless Facility, McCafe, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1636,6 +1846,11 @@
       <c r="F43" t="n">
         <v>101.744674130684</v>
       </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Drive-Thru, Breakfast, Cashless Facility, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1664,6 +1879,11 @@
       <c r="F44" t="n">
         <v>101.7086</v>
       </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Drive-Thru, Breakfast, Cashless Facility, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1692,6 +1912,11 @@
       <c r="F45" t="n">
         <v>101.65492</v>
       </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>24 Hours, Drive-Thru, Breakfast, Cashless Facility, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1720,6 +1945,11 @@
       <c r="F46" t="n">
         <v>101.666333</v>
       </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Drive-Thru, Breakfast, Cashless Facility, McCafe, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1744,6 +1974,11 @@
       <c r="F47" t="n">
         <v>101.7137842</v>
       </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Drive-Thru, Breakfast, Cashless Facility, McCafe, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1772,6 +2007,11 @@
       <c r="F48" t="n">
         <v>101.7515586</v>
       </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Drive-Thru, Breakfast, Cashless Facility, McCafe, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1800,6 +2040,11 @@
       <c r="F49" t="n">
         <v>101.700383</v>
       </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Breakfast, Cashless Facility, McCafe, WiFi, Digital Order Kiosk, Surau</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1824,6 +2069,11 @@
       <c r="F50" t="n">
         <v>101.70641</v>
       </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>24 Hours, Birthday Party, Drive-Thru, Breakfast, Cashless Facility, McCafe, McDelivery, WiFi, Digital Order Kiosk</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1852,6 +2102,11 @@
       <c r="F51" t="n">
         <v>101.686130313856</v>
       </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Drive-Thru, Breakfast, Cashless Facility, McCafe, WiFi, Digital Order Kiosk, Surau</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1875,6 +2130,11 @@
       </c>
       <c r="F52" t="n">
         <v>101.700753</v>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Breakfast, Cashless Facility, McCafe, WiFi, Digital Order Kiosk</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>